<commit_message>
fix(bipumin.xlsx): 비품인 엑셀 양식 변경
</commit_message>
<xml_diff>
--- a/public/data/bipumin.xlsx
+++ b/public/data/bipumin.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="현재_통합_문서"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seogun/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seogun/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8D0B462-63A2-FE41-B81E-BB7317FB32AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCF88063-BE73-6F40-88DD-AAA9B0213FB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,114 +31,115 @@
     <t>사용자</t>
   </si>
   <si>
+    <t>비품관리대장</t>
+  </si>
+  <si>
+    <t>등록일자</t>
+  </si>
+  <si>
+    <t>협력업체</t>
+  </si>
+  <si>
+    <t>삼성 오디세이 게이밍 모니터</t>
+  </si>
+  <si>
+    <t>제품명</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>시리얼 넘버</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>등록일자</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>부서</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>사용자</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>협력업체</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>항목</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>항목별 주의 사항</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>30자 이내로만 입력이 가능</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>yyyy.mm.dd 의 형식으로 작성</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>등록된 소분류 카테고리만 입력 가능</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>등록된 부서와 일치하는 사원명만 입력 가능</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>등록된 부서만 입력 가능</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>등록된 협력업체만 입력 가능</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>공백</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>개인 비품</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>공용 비품</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>공용 비품 등록시 사용자 항목은 공백으로 처리해주세요.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>개발팀</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>종류</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>모니터</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MO2463453</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>엑셀을 통한 복수 등록시, 2개 이상부터 등록이 가능하며, 종류, 제품명, 시리얼 넘버는 필수 입니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>새로운 시트를 추가할때는 해당 시트를 복사 후 사용해주세요.</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
     <t>시리얼넘버</t>
-  </si>
-  <si>
-    <t>비품관리대장</t>
-  </si>
-  <si>
-    <t>등록일자</t>
-  </si>
-  <si>
-    <t>협력업체</t>
-  </si>
-  <si>
-    <t>삼성 오디세이 게이밍 모니터</t>
-  </si>
-  <si>
-    <t>제품명</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>시리얼 넘버</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>등록일자</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>부서</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>사용자</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>협력업체</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>항목</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>항목별 주의 사항</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>30자 이내로만 입력이 가능</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>yyyy.mm.dd 의 형식으로 작성</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>등록된 소분류 카테고리만 입력 가능</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>등록된 부서와 일치하는 사원명만 입력 가능</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>등록된 부서만 입력 가능</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>등록된 협력업체만 입력 가능</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>공백</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>개인 비품</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>공용 비품</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>공용 비품 등록시 사용자 항목은 공백으로 처리해주세요.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>개발팀</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>종류</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>모니터</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>MO2463453</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>엑셀을 통한 복수 등록시, 2개 이상부터 등록이 가능하며, 종류, 제품명, 시리얼 넘버는 필수 입니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>새로운 시트를 추가할때는 해당 시트를 복사 후 사용해주세요.</t>
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
 </sst>
@@ -920,8 +921,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20E8C7FC-ADAF-8144-A267-7870FD173818}">
   <dimension ref="A1:O46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="110" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="20" customHeight="1"/>
@@ -976,7 +977,7 @@
     </row>
     <row r="4" spans="1:12" ht="20" customHeight="1">
       <c r="A4" s="32" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="33"/>
       <c r="C4" s="33"/>
@@ -1021,7 +1022,7 @@
       <c r="A8" s="9"/>
       <c r="B8" s="9"/>
       <c r="C8" s="38" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D8" s="38"/>
       <c r="E8" s="38"/>
@@ -1033,7 +1034,7 @@
       <c r="A9" s="9"/>
       <c r="B9" s="9"/>
       <c r="C9" s="39" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D9" s="39"/>
       <c r="E9" s="39"/>
@@ -1045,7 +1046,7 @@
       <c r="A10" s="9"/>
       <c r="B10" s="9"/>
       <c r="C10" s="39" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D10" s="39"/>
       <c r="E10" s="39"/>
@@ -1067,13 +1068,13 @@
       <c r="A12" s="9"/>
       <c r="B12" s="16"/>
       <c r="C12" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D12" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="17" t="s">
         <v>23</v>
-      </c>
-      <c r="E12" s="17" t="s">
-        <v>24</v>
       </c>
       <c r="F12" s="9"/>
       <c r="G12" s="14"/>
@@ -1083,10 +1084,10 @@
       <c r="A13" s="9"/>
       <c r="B13" s="16"/>
       <c r="C13" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D13" s="30" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E13" s="30"/>
       <c r="F13" s="9"/>
@@ -1097,10 +1098,10 @@
       <c r="A14" s="9"/>
       <c r="B14" s="16"/>
       <c r="C14" s="18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D14" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E14" s="30"/>
       <c r="F14" s="9"/>
@@ -1111,7 +1112,7 @@
       <c r="A15" s="9"/>
       <c r="B15" s="16"/>
       <c r="C15" s="18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D15" s="30"/>
       <c r="E15" s="30"/>
@@ -1123,10 +1124,10 @@
       <c r="A16" s="9"/>
       <c r="B16" s="16"/>
       <c r="C16" s="19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D16" s="30" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E16" s="30"/>
       <c r="F16" s="9"/>
@@ -1137,10 +1138,10 @@
       <c r="A17" s="9"/>
       <c r="B17" s="16"/>
       <c r="C17" s="19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D17" s="30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E17" s="30"/>
       <c r="F17" s="9"/>
@@ -1151,13 +1152,13 @@
       <c r="A18" s="9"/>
       <c r="B18" s="16"/>
       <c r="C18" s="19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E18" s="20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F18" s="9"/>
       <c r="G18" s="14"/>
@@ -1167,10 +1168,10 @@
       <c r="A19" s="9"/>
       <c r="B19" s="9"/>
       <c r="C19" s="19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D19" s="30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E19" s="30"/>
       <c r="F19" s="9"/>
@@ -1181,7 +1182,7 @@
       <c r="A20" s="9"/>
       <c r="B20" s="16"/>
       <c r="C20" s="40" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D20" s="40"/>
       <c r="E20" s="40"/>
@@ -1201,16 +1202,16 @@
     </row>
     <row r="22" spans="1:15" ht="36" customHeight="1">
       <c r="A22" s="21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B22" s="22" t="s">
         <v>1</v>
       </c>
       <c r="C22" s="22" t="s">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="D22" s="23" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E22" s="23" t="s">
         <v>0</v>
@@ -1219,7 +1220,7 @@
         <v>2</v>
       </c>
       <c r="G22" s="24" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I22" s="11"/>
       <c r="J22" s="11"/>
@@ -1231,19 +1232,19 @@
     </row>
     <row r="23" spans="1:15" ht="20" customHeight="1">
       <c r="A23" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="D23" s="28">
         <v>44673</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I23" s="11"/>
     </row>
@@ -1398,7 +1399,7 @@
       <c r="O46" s="11"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="X3d23LlSUtO854zQ93YnWocx1wLMqrPCAhUElPSlqN4cAu1qQ62V5spT5sWLeEQMDifGseg50CZ+yBs/Puv4gg==" saltValue="6DadtDcJaX/E/qLVxTl/vg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="11">
     <mergeCell ref="D14:E15"/>
     <mergeCell ref="D16:E16"/>

</xml_diff>